<commit_message>
can add/update jobs now
</commit_message>
<xml_diff>
--- a/ICS4U7 IA - Data Porter/bin/farms4life2016/init/initialization.xlsx
+++ b/ICS4U7 IA - Data Porter/bin/farms4life2016/init/initialization.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
   <si>
     <t>Id</t>
   </si>
@@ -44,7 +44,7 @@
     <t>I_Supplier.xml</t>
   </si>
   <si>
-    <t>Feb 11, 2022 (09:55:41 EST)</t>
+    <t>Feb 12, 2022 (01:18:16 EST)</t>
   </si>
   <si>
     <t>Plant</t>
@@ -53,6 +53,9 @@
     <t>I_Plant.xml</t>
   </si>
   <si>
+    <t>Feb 12, 2022 (01:18:09 EST)</t>
+  </si>
+  <si>
     <t>Solicitation</t>
   </si>
   <si>
@@ -74,7 +77,13 @@
     <t>E_RequestFile.xml</t>
   </si>
   <si>
+    <t>BOMB</t>
+  </si>
+  <si>
     <t>E_BOM.xml</t>
+  </si>
+  <si>
+    <t>Feb 12, 2022 (01:18:29 EST)</t>
   </si>
   <si>
     <t>GYU</t>
@@ -185,7 +194,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -193,7 +202,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -202,10 +211,10 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -213,7 +222,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -222,10 +231,10 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -233,19 +242,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -253,19 +262,19 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
@@ -276,7 +285,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -285,7 +294,7 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -296,7 +305,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -305,7 +314,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -313,19 +322,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -333,19 +342,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -353,19 +362,19 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -373,19 +382,19 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved some stuff, changed to java 1.8
</commit_message>
<xml_diff>
--- a/ICS4U7 IA - Data Porter/bin/farms4life2016/init/initialization.xlsx
+++ b/ICS4U7 IA - Data Porter/bin/farms4life2016/init/initialization.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
   <si>
     <t>Id</t>
   </si>
@@ -44,7 +44,7 @@
     <t>I_Supplier.xml</t>
   </si>
   <si>
-    <t>Feb 12, 2022 (01:18:16 EST)</t>
+    <t>Feb 12, 2022 (04:14:47 EST)</t>
   </si>
   <si>
     <t>Plant</t>
@@ -53,9 +53,6 @@
     <t>I_Plant.xml</t>
   </si>
   <si>
-    <t>Feb 12, 2022 (01:18:09 EST)</t>
-  </si>
-  <si>
     <t>Solicitation</t>
   </si>
   <si>
@@ -77,13 +74,7 @@
     <t>E_RequestFile.xml</t>
   </si>
   <si>
-    <t>BOMB</t>
-  </si>
-  <si>
     <t>E_BOM.xml</t>
-  </si>
-  <si>
-    <t>Feb 12, 2022 (01:18:29 EST)</t>
   </si>
   <si>
     <t>GYU</t>
@@ -194,7 +185,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -202,19 +193,19 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -222,19 +213,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -242,19 +233,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -262,19 +253,19 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -285,7 +276,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -294,7 +285,7 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -305,7 +296,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -314,7 +305,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -322,19 +313,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -342,19 +333,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -362,19 +353,19 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" t="s">
-        <v>20</v>
-      </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -382,19 +373,19 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>